<commit_message>
27th of March Update 1
</commit_message>
<xml_diff>
--- a/docs/Netlist_1.xlsx
+++ b/docs/Netlist_1.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Netlist_1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" refMode="R1C1"/>
+  <calcPr calcId="125725" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1631" uniqueCount="806">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1633" uniqueCount="808">
   <si>
     <t>РљРѕРґ С†РµРїРё</t>
   </si>
@@ -2432,6 +2432,12 @@
   </si>
   <si>
     <t>Блок Д1 развернуть</t>
+  </si>
+  <si>
+    <t>U66 РАЗВЕРНУТЬ!</t>
+  </si>
+  <si>
+    <t>сейчас третий пин порта, ждолжен быть первый, вход магнитофона идет на 20, выход на 21</t>
   </si>
 </sst>
 </file>
@@ -3294,8 +3300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K325"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3967,7 +3973,7 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C26">
@@ -3993,7 +3999,7 @@
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C27">
@@ -4019,7 +4025,7 @@
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>76</v>
       </c>
       <c r="C28">
@@ -4045,7 +4051,7 @@
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C29">
@@ -4071,7 +4077,7 @@
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>81</v>
       </c>
       <c r="C30">
@@ -4097,7 +4103,7 @@
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>83</v>
       </c>
       <c r="C31">
@@ -4123,7 +4129,7 @@
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C32">
@@ -4149,7 +4155,7 @@
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C33">
@@ -4175,7 +4181,7 @@
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C34">
@@ -4201,7 +4207,7 @@
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C35">
@@ -4227,7 +4233,7 @@
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="1" t="s">
         <v>94</v>
       </c>
       <c r="C36">
@@ -4253,7 +4259,7 @@
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="1" t="s">
         <v>96</v>
       </c>
       <c r="C37">
@@ -4279,7 +4285,7 @@
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="2" t="s">
         <v>98</v>
       </c>
       <c r="C38">
@@ -4305,7 +4311,7 @@
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="1" t="s">
         <v>101</v>
       </c>
       <c r="C39">
@@ -4331,7 +4337,7 @@
       <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="2" t="s">
         <v>103</v>
       </c>
       <c r="C40">
@@ -4357,7 +4363,7 @@
       <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="1" t="s">
         <v>105</v>
       </c>
       <c r="C41">
@@ -4383,7 +4389,7 @@
       <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="2" t="s">
         <v>106</v>
       </c>
       <c r="C42">
@@ -4409,7 +4415,7 @@
       <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C43">
@@ -4435,7 +4441,7 @@
       <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="1" t="s">
         <v>110</v>
       </c>
       <c r="C44">
@@ -4461,7 +4467,7 @@
       <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C45">
@@ -4487,7 +4493,7 @@
       <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C46">
@@ -4513,7 +4519,7 @@
       <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="1" t="s">
         <v>117</v>
       </c>
       <c r="C47">
@@ -4539,7 +4545,7 @@
       <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="1" t="s">
         <v>119</v>
       </c>
       <c r="C48">
@@ -4565,7 +4571,7 @@
       <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="1" t="s">
         <v>121</v>
       </c>
       <c r="C49">
@@ -4591,7 +4597,7 @@
       <c r="A50">
         <v>49</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="1" t="s">
         <v>123</v>
       </c>
       <c r="C50">
@@ -4617,7 +4623,7 @@
       <c r="A51">
         <v>50</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C51">
@@ -4643,7 +4649,7 @@
       <c r="A52">
         <v>51</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="1" t="s">
         <v>128</v>
       </c>
       <c r="C52">
@@ -4669,7 +4675,7 @@
       <c r="A53">
         <v>52</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="1" t="s">
         <v>131</v>
       </c>
       <c r="C53">
@@ -4695,7 +4701,7 @@
       <c r="A54">
         <v>53</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="1" t="s">
         <v>133</v>
       </c>
       <c r="C54">
@@ -4721,7 +4727,7 @@
       <c r="A55">
         <v>54</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="1" t="s">
         <v>134</v>
       </c>
       <c r="C55">
@@ -4747,7 +4753,7 @@
       <c r="A56">
         <v>55</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="1" t="s">
         <v>136</v>
       </c>
       <c r="C56">
@@ -4773,7 +4779,7 @@
       <c r="A57">
         <v>56</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="1" t="s">
         <v>138</v>
       </c>
       <c r="C57">
@@ -4799,7 +4805,7 @@
       <c r="A58">
         <v>57</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="1" t="s">
         <v>140</v>
       </c>
       <c r="C58">
@@ -4825,7 +4831,7 @@
       <c r="A59">
         <v>58</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="3" t="s">
         <v>141</v>
       </c>
       <c r="C59">
@@ -4851,7 +4857,7 @@
       <c r="A60">
         <v>59</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="1" t="s">
         <v>145</v>
       </c>
       <c r="C60">
@@ -4877,7 +4883,7 @@
       <c r="A61">
         <v>60</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="1" t="s">
         <v>147</v>
       </c>
       <c r="C61">
@@ -4903,7 +4909,7 @@
       <c r="A62">
         <v>61</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="1" t="s">
         <v>149</v>
       </c>
       <c r="C62">
@@ -4929,7 +4935,7 @@
       <c r="A63">
         <v>62</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="1" t="s">
         <v>151</v>
       </c>
       <c r="C63">
@@ -4955,7 +4961,7 @@
       <c r="A64">
         <v>63</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="1" t="s">
         <v>153</v>
       </c>
       <c r="C64">
@@ -4977,11 +4983,11 @@
         <v>154</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:10">
       <c r="A65">
         <v>64</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="1" t="s">
         <v>155</v>
       </c>
       <c r="C65">
@@ -5003,11 +5009,11 @@
         <v>156</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:10">
       <c r="A66">
         <v>65</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="1" t="s">
         <v>157</v>
       </c>
       <c r="C66">
@@ -5029,11 +5035,11 @@
         <v>158</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:10">
       <c r="A67">
         <v>66</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="1" t="s">
         <v>159</v>
       </c>
       <c r="C67">
@@ -5055,11 +5061,11 @@
         <v>160</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:10">
       <c r="A68">
         <v>67</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="1" t="s">
         <v>161</v>
       </c>
       <c r="C68">
@@ -5081,11 +5087,11 @@
         <v>162</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:10">
       <c r="A69">
         <v>68</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="3" t="s">
         <v>163</v>
       </c>
       <c r="C69">
@@ -5106,12 +5112,15 @@
       <c r="H69" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="70" spans="1:8">
+      <c r="J69" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
       <c r="A70">
         <v>69</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="1" t="s">
         <v>167</v>
       </c>
       <c r="C70">
@@ -5133,11 +5142,11 @@
         <v>169</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:10">
       <c r="A71">
         <v>70</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="1" t="s">
         <v>170</v>
       </c>
       <c r="C71">
@@ -5159,11 +5168,11 @@
         <v>171</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:10">
       <c r="A72">
         <v>71</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="1" t="s">
         <v>172</v>
       </c>
       <c r="C72">
@@ -5185,11 +5194,11 @@
         <v>174</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:10">
       <c r="A73">
         <v>72</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="1" t="s">
         <v>175</v>
       </c>
       <c r="C73">
@@ -5211,11 +5220,11 @@
         <v>177</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:10">
       <c r="A74">
         <v>73</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="1" t="s">
         <v>178</v>
       </c>
       <c r="C74">
@@ -5237,11 +5246,11 @@
         <v>180</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:10">
       <c r="A75">
         <v>74</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="1" t="s">
         <v>181</v>
       </c>
       <c r="C75">
@@ -5263,11 +5272,11 @@
         <v>183</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:10">
       <c r="A76">
         <v>75</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="1" t="s">
         <v>184</v>
       </c>
       <c r="C76">
@@ -5289,11 +5298,11 @@
         <v>186</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:10">
       <c r="A77">
         <v>76</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="1" t="s">
         <v>187</v>
       </c>
       <c r="C77">
@@ -5315,11 +5324,11 @@
         <v>189</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:10">
       <c r="A78">
         <v>77</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="2" t="s">
         <v>190</v>
       </c>
       <c r="C78">
@@ -5340,12 +5349,15 @@
       <c r="H78" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="79" spans="1:8">
+      <c r="J78" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
       <c r="A79">
         <v>78</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="1" t="s">
         <v>192</v>
       </c>
       <c r="C79">
@@ -5367,11 +5379,11 @@
         <v>193</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:10">
       <c r="A80">
         <v>79</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="2" t="s">
         <v>194</v>
       </c>
       <c r="C80">
@@ -5397,7 +5409,7 @@
       <c r="A81">
         <v>83</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="1" t="s">
         <v>196</v>
       </c>
       <c r="C81">
@@ -5423,7 +5435,7 @@
       <c r="A82">
         <v>84</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="1" t="s">
         <v>198</v>
       </c>
       <c r="C82">
@@ -5449,7 +5461,7 @@
       <c r="A83">
         <v>85</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="1" t="s">
         <v>200</v>
       </c>
       <c r="C83">
@@ -5475,7 +5487,7 @@
       <c r="A84">
         <v>86</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="1" t="s">
         <v>202</v>
       </c>
       <c r="C84">
@@ -5501,7 +5513,7 @@
       <c r="A85">
         <v>87</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="3" t="s">
         <v>204</v>
       </c>
       <c r="C85">
@@ -5527,7 +5539,7 @@
       <c r="A86">
         <v>88</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="3" t="s">
         <v>206</v>
       </c>
       <c r="C86">
@@ -5553,7 +5565,7 @@
       <c r="A87">
         <v>89</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="1" t="s">
         <v>208</v>
       </c>
       <c r="C87">
@@ -5579,7 +5591,7 @@
       <c r="A88">
         <v>90</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="1" t="s">
         <v>211</v>
       </c>
       <c r="C88">
@@ -5605,7 +5617,7 @@
       <c r="A89">
         <v>91</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="1" t="s">
         <v>213</v>
       </c>
       <c r="C89">
@@ -5631,7 +5643,7 @@
       <c r="A90">
         <v>92</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="1" t="s">
         <v>215</v>
       </c>
       <c r="C90">
@@ -5657,7 +5669,7 @@
       <c r="A91">
         <v>93</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="1" t="s">
         <v>218</v>
       </c>
       <c r="C91">
@@ -5683,7 +5695,7 @@
       <c r="A92">
         <v>94</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="1" t="s">
         <v>221</v>
       </c>
       <c r="C92">
@@ -5709,7 +5721,7 @@
       <c r="A93">
         <v>95</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="1" t="s">
         <v>223</v>
       </c>
       <c r="C93">
@@ -5735,7 +5747,7 @@
       <c r="A94">
         <v>96</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="1" t="s">
         <v>225</v>
       </c>
       <c r="C94">
@@ -5761,7 +5773,7 @@
       <c r="A95">
         <v>97</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="1" t="s">
         <v>227</v>
       </c>
       <c r="C95">
@@ -5787,7 +5799,7 @@
       <c r="A96">
         <v>98</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="1" t="s">
         <v>229</v>
       </c>
       <c r="C96">
@@ -5813,7 +5825,7 @@
       <c r="A97">
         <v>99</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="1" t="s">
         <v>231</v>
       </c>
       <c r="C97">
@@ -5839,7 +5851,7 @@
       <c r="A98">
         <v>100</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="1" t="s">
         <v>233</v>
       </c>
       <c r="C98">
@@ -5865,7 +5877,7 @@
       <c r="A99">
         <v>101</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="1" t="s">
         <v>235</v>
       </c>
       <c r="C99">
@@ -11765,5 +11777,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
29th march 2023 Update 1
</commit_message>
<xml_diff>
--- a/docs/Netlist_1.xlsx
+++ b/docs/Netlist_1.xlsx
@@ -2434,10 +2434,10 @@
     <t>Блок Д1 развернуть</t>
   </si>
   <si>
-    <t>U66 РАЗВЕРНУТЬ!</t>
-  </si>
-  <si>
     <t>сейчас третий пин порта, ждолжен быть первый, вход магнитофона идет на 20, выход на 21</t>
+  </si>
+  <si>
+    <t>перевернуть R35</t>
   </si>
 </sst>
 </file>
@@ -3300,8 +3300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K325"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B122" sqref="B122"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I74" sqref="I74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -5112,9 +5112,6 @@
       <c r="H69" t="s">
         <v>166</v>
       </c>
-      <c r="J69" t="s">
-        <v>806</v>
-      </c>
     </row>
     <row r="70" spans="1:10">
       <c r="A70">
@@ -5350,7 +5347,7 @@
         <v>191</v>
       </c>
       <c r="J78" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -6237,7 +6234,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:10">
       <c r="A113">
         <v>115</v>
       </c>
@@ -6263,7 +6260,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:10">
       <c r="A114">
         <v>116</v>
       </c>
@@ -6289,7 +6286,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:10">
       <c r="A115">
         <v>117</v>
       </c>
@@ -6315,7 +6312,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:10">
       <c r="A116">
         <v>118</v>
       </c>
@@ -6341,7 +6338,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:10">
       <c r="A117">
         <v>119</v>
       </c>
@@ -6367,7 +6364,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:10">
       <c r="A118">
         <v>120</v>
       </c>
@@ -6393,11 +6390,11 @@
         <v>285</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:10">
       <c r="A119">
         <v>121</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B119" s="1" t="s">
         <v>286</v>
       </c>
       <c r="C119">
@@ -6419,11 +6416,11 @@
         <v>287</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:10">
       <c r="A120">
         <v>122</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B120" s="1" t="s">
         <v>288</v>
       </c>
       <c r="C120">
@@ -6445,37 +6442,40 @@
         <v>289</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
-      <c r="A121">
+    <row r="121" spans="1:10" s="2" customFormat="1">
+      <c r="A121" s="2">
         <v>123</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B121" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="C121">
-        <v>2</v>
-      </c>
-      <c r="D121">
-        <v>0</v>
-      </c>
-      <c r="E121" t="s">
-        <v>9</v>
-      </c>
-      <c r="F121" t="s">
+      <c r="C121" s="2">
+        <v>2</v>
+      </c>
+      <c r="D121" s="2">
+        <v>0</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F121" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="G121" t="s">
-        <v>9</v>
-      </c>
-      <c r="H121" t="s">
+      <c r="G121" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H121" s="2" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="122" spans="1:8">
+      <c r="J121" s="2" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10">
       <c r="A122">
         <v>124</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B122" s="1" t="s">
         <v>292</v>
       </c>
       <c r="C122">
@@ -6497,11 +6497,11 @@
         <v>293</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:10">
       <c r="A123">
         <v>125</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B123" s="1" t="s">
         <v>294</v>
       </c>
       <c r="C123">
@@ -6523,37 +6523,37 @@
         <v>295</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
-      <c r="A124">
+    <row r="124" spans="1:10" s="2" customFormat="1">
+      <c r="A124" s="2">
         <v>126</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B124" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="C124">
+      <c r="C124" s="2">
         <v>6</v>
       </c>
-      <c r="D124">
-        <v>0</v>
-      </c>
-      <c r="E124" t="s">
-        <v>9</v>
-      </c>
-      <c r="F124" t="s">
+      <c r="D124" s="2">
+        <v>0</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F124" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="G124" t="s">
-        <v>9</v>
-      </c>
-      <c r="H124" t="s">
+      <c r="G124" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H124" s="2" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:10">
       <c r="A125">
         <v>127</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B125" s="1" t="s">
         <v>298</v>
       </c>
       <c r="C125">
@@ -6575,11 +6575,11 @@
         <v>299</v>
       </c>
     </row>
-    <row r="126" spans="1:8">
+    <row r="126" spans="1:10">
       <c r="A126">
         <v>128</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B126" s="1" t="s">
         <v>300</v>
       </c>
       <c r="C126">
@@ -6601,11 +6601,11 @@
         <v>301</v>
       </c>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:10">
       <c r="A127">
         <v>129</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B127" s="1" t="s">
         <v>302</v>
       </c>
       <c r="C127">
@@ -6627,11 +6627,11 @@
         <v>303</v>
       </c>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:10">
       <c r="A128">
         <v>130</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B128" s="1" t="s">
         <v>304</v>
       </c>
       <c r="C128">
@@ -6657,7 +6657,7 @@
       <c r="A129">
         <v>131</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B129" s="1" t="s">
         <v>306</v>
       </c>
       <c r="C129">
@@ -6683,7 +6683,7 @@
       <c r="A130">
         <v>132</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B130" s="1" t="s">
         <v>308</v>
       </c>
       <c r="C130">
@@ -6709,7 +6709,7 @@
       <c r="A131">
         <v>133</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B131" s="1" t="s">
         <v>311</v>
       </c>
       <c r="C131">
@@ -6735,7 +6735,7 @@
       <c r="A132">
         <v>134</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B132" s="1" t="s">
         <v>314</v>
       </c>
       <c r="C132">
@@ -6761,7 +6761,7 @@
       <c r="A133">
         <v>138</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B133" s="1" t="s">
         <v>316</v>
       </c>
       <c r="C133">
@@ -6787,7 +6787,7 @@
       <c r="A134">
         <v>139</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B134" s="1" t="s">
         <v>318</v>
       </c>
       <c r="C134">
@@ -6813,7 +6813,7 @@
       <c r="A135">
         <v>140</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B135" s="1" t="s">
         <v>321</v>
       </c>
       <c r="C135">
@@ -6839,7 +6839,7 @@
       <c r="A136">
         <v>141</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B136" s="1" t="s">
         <v>324</v>
       </c>
       <c r="C136">
@@ -6865,7 +6865,7 @@
       <c r="A137">
         <v>142</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B137" s="1" t="s">
         <v>326</v>
       </c>
       <c r="C137">
@@ -6891,7 +6891,7 @@
       <c r="A138">
         <v>143</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B138" s="1" t="s">
         <v>328</v>
       </c>
       <c r="C138">
@@ -6917,7 +6917,7 @@
       <c r="A139">
         <v>144</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B139" s="1" t="s">
         <v>330</v>
       </c>
       <c r="C139">
@@ -6943,7 +6943,7 @@
       <c r="A140">
         <v>145</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B140" s="1" t="s">
         <v>332</v>
       </c>
       <c r="C140">
@@ -6969,7 +6969,7 @@
       <c r="A141">
         <v>148</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B141" s="1" t="s">
         <v>335</v>
       </c>
       <c r="C141">
@@ -6995,7 +6995,7 @@
       <c r="A142">
         <v>149</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B142" s="1" t="s">
         <v>338</v>
       </c>
       <c r="C142">
@@ -7021,7 +7021,7 @@
       <c r="A143">
         <v>150</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B143" s="1" t="s">
         <v>341</v>
       </c>
       <c r="C143">
@@ -7047,7 +7047,7 @@
       <c r="A144">
         <v>151</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B144" s="1" t="s">
         <v>344</v>
       </c>
       <c r="C144">
@@ -7073,7 +7073,7 @@
       <c r="A145">
         <v>152</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B145" s="1" t="s">
         <v>347</v>
       </c>
       <c r="C145">
@@ -7099,7 +7099,7 @@
       <c r="A146">
         <v>154</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B146" s="1" t="s">
         <v>350</v>
       </c>
       <c r="C146">
@@ -7125,7 +7125,7 @@
       <c r="A147">
         <v>155</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B147" s="1" t="s">
         <v>352</v>
       </c>
       <c r="C147">
@@ -7151,7 +7151,7 @@
       <c r="A148">
         <v>156</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B148" s="1" t="s">
         <v>354</v>
       </c>
       <c r="C148">
@@ -7177,7 +7177,7 @@
       <c r="A149">
         <v>159</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B149" s="1" t="s">
         <v>356</v>
       </c>
       <c r="C149">
@@ -7203,7 +7203,7 @@
       <c r="A150">
         <v>161</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B150" s="1" t="s">
         <v>358</v>
       </c>
       <c r="C150">
@@ -7229,7 +7229,7 @@
       <c r="A151">
         <v>162</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B151" s="1" t="s">
         <v>361</v>
       </c>
       <c r="C151">
@@ -7255,7 +7255,7 @@
       <c r="A152">
         <v>163</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B152" s="1" t="s">
         <v>364</v>
       </c>
       <c r="C152">
@@ -7281,7 +7281,7 @@
       <c r="A153">
         <v>164</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B153" s="1" t="s">
         <v>367</v>
       </c>
       <c r="C153">
@@ -7307,7 +7307,7 @@
       <c r="A154">
         <v>166</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B154" s="1" t="s">
         <v>370</v>
       </c>
       <c r="C154">
@@ -7333,7 +7333,7 @@
       <c r="A155">
         <v>167</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B155" s="1" t="s">
         <v>373</v>
       </c>
       <c r="C155">
@@ -7359,7 +7359,7 @@
       <c r="A156">
         <v>170</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B156" s="1" t="s">
         <v>375</v>
       </c>
       <c r="C156">
@@ -7385,7 +7385,7 @@
       <c r="A157">
         <v>171</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B157" s="1" t="s">
         <v>377</v>
       </c>
       <c r="C157">
@@ -7411,7 +7411,7 @@
       <c r="A158">
         <v>172</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B158" s="1" t="s">
         <v>379</v>
       </c>
       <c r="C158">
@@ -7437,7 +7437,7 @@
       <c r="A159">
         <v>173</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B159" s="1" t="s">
         <v>381</v>
       </c>
       <c r="C159">
@@ -7463,7 +7463,7 @@
       <c r="A160">
         <v>175</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B160" s="1" t="s">
         <v>384</v>
       </c>
       <c r="C160">
@@ -7489,7 +7489,7 @@
       <c r="A161">
         <v>176</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B161" s="1" t="s">
         <v>387</v>
       </c>
       <c r="C161">
@@ -7515,7 +7515,7 @@
       <c r="A162">
         <v>177</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B162" s="1" t="s">
         <v>389</v>
       </c>
       <c r="C162">
@@ -7541,7 +7541,7 @@
       <c r="A163">
         <v>178</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B163" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C163">
@@ -7567,7 +7567,7 @@
       <c r="A164">
         <v>179</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B164" s="1" t="s">
         <v>394</v>
       </c>
       <c r="C164">
@@ -7593,7 +7593,7 @@
       <c r="A165">
         <v>180</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B165" s="1" t="s">
         <v>396</v>
       </c>
       <c r="C165">
@@ -7619,7 +7619,7 @@
       <c r="A166">
         <v>181</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B166" s="1" t="s">
         <v>398</v>
       </c>
       <c r="C166">
@@ -7645,7 +7645,7 @@
       <c r="A167">
         <v>182</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B167" s="1" t="s">
         <v>400</v>
       </c>
       <c r="C167">
@@ -7671,7 +7671,7 @@
       <c r="A168">
         <v>183</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B168" s="1" t="s">
         <v>402</v>
       </c>
       <c r="C168">
@@ -7697,7 +7697,7 @@
       <c r="A169">
         <v>184</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B169" s="1" t="s">
         <v>404</v>
       </c>
       <c r="C169">
@@ -7723,7 +7723,7 @@
       <c r="A170">
         <v>185</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B170" s="1" t="s">
         <v>406</v>
       </c>
       <c r="C170">
@@ -7749,7 +7749,7 @@
       <c r="A171">
         <v>186</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B171" s="1" t="s">
         <v>408</v>
       </c>
       <c r="C171">
@@ -7775,7 +7775,7 @@
       <c r="A172">
         <v>187</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B172" s="1" t="s">
         <v>411</v>
       </c>
       <c r="C172">
@@ -7801,7 +7801,7 @@
       <c r="A173">
         <v>188</v>
       </c>
-      <c r="B173" t="s">
+      <c r="B173" s="1" t="s">
         <v>413</v>
       </c>
       <c r="C173">
@@ -7827,7 +7827,7 @@
       <c r="A174">
         <v>189</v>
       </c>
-      <c r="B174" t="s">
+      <c r="B174" s="1" t="s">
         <v>415</v>
       </c>
       <c r="C174">
@@ -7853,7 +7853,7 @@
       <c r="A175">
         <v>190</v>
       </c>
-      <c r="B175" t="s">
+      <c r="B175" s="1" t="s">
         <v>418</v>
       </c>
       <c r="C175">
@@ -7879,7 +7879,7 @@
       <c r="A176">
         <v>194</v>
       </c>
-      <c r="B176" t="s">
+      <c r="B176" s="1" t="s">
         <v>421</v>
       </c>
       <c r="C176">
@@ -7905,7 +7905,7 @@
       <c r="A177">
         <v>195</v>
       </c>
-      <c r="B177" t="s">
+      <c r="B177" s="1" t="s">
         <v>423</v>
       </c>
       <c r="C177">
@@ -7931,7 +7931,7 @@
       <c r="A178">
         <v>199</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B178" s="1" t="s">
         <v>426</v>
       </c>
       <c r="C178">
@@ -7957,7 +7957,7 @@
       <c r="A179">
         <v>200</v>
       </c>
-      <c r="B179" t="s">
+      <c r="B179" s="1" t="s">
         <v>428</v>
       </c>
       <c r="C179">
@@ -7983,7 +7983,7 @@
       <c r="A180">
         <v>201</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B180" s="1" t="s">
         <v>431</v>
       </c>
       <c r="C180">
@@ -8009,7 +8009,7 @@
       <c r="A181">
         <v>202</v>
       </c>
-      <c r="B181" t="s">
+      <c r="B181" s="1" t="s">
         <v>434</v>
       </c>
       <c r="C181">
@@ -8035,7 +8035,7 @@
       <c r="A182">
         <v>209</v>
       </c>
-      <c r="B182" t="s">
+      <c r="B182" s="1" t="s">
         <v>437</v>
       </c>
       <c r="C182">
@@ -8061,7 +8061,7 @@
       <c r="A183">
         <v>210</v>
       </c>
-      <c r="B183" t="s">
+      <c r="B183" s="1" t="s">
         <v>439</v>
       </c>
       <c r="C183">
@@ -8087,7 +8087,7 @@
       <c r="A184">
         <v>211</v>
       </c>
-      <c r="B184" t="s">
+      <c r="B184" s="1" t="s">
         <v>442</v>
       </c>
       <c r="C184">
@@ -8113,7 +8113,7 @@
       <c r="A185">
         <v>212</v>
       </c>
-      <c r="B185" t="s">
+      <c r="B185" s="1" t="s">
         <v>445</v>
       </c>
       <c r="C185">
@@ -8139,7 +8139,7 @@
       <c r="A186">
         <v>213</v>
       </c>
-      <c r="B186" t="s">
+      <c r="B186" s="1" t="s">
         <v>448</v>
       </c>
       <c r="C186">
@@ -8165,7 +8165,7 @@
       <c r="A187">
         <v>217</v>
       </c>
-      <c r="B187" t="s">
+      <c r="B187" s="1" t="s">
         <v>450</v>
       </c>
       <c r="C187">
@@ -8191,7 +8191,7 @@
       <c r="A188">
         <v>218</v>
       </c>
-      <c r="B188" t="s">
+      <c r="B188" s="1" t="s">
         <v>453</v>
       </c>
       <c r="C188">
@@ -8217,7 +8217,7 @@
       <c r="A189">
         <v>219</v>
       </c>
-      <c r="B189" t="s">
+      <c r="B189" s="1" t="s">
         <v>455</v>
       </c>
       <c r="C189">
@@ -8243,7 +8243,7 @@
       <c r="A190">
         <v>220</v>
       </c>
-      <c r="B190" t="s">
+      <c r="B190" s="1" t="s">
         <v>457</v>
       </c>
       <c r="C190">
@@ -8269,7 +8269,7 @@
       <c r="A191">
         <v>221</v>
       </c>
-      <c r="B191" t="s">
+      <c r="B191" s="1" t="s">
         <v>459</v>
       </c>
       <c r="C191">
@@ -8295,7 +8295,7 @@
       <c r="A192">
         <v>222</v>
       </c>
-      <c r="B192" t="s">
+      <c r="B192" s="1" t="s">
         <v>462</v>
       </c>
       <c r="C192">
@@ -8321,7 +8321,7 @@
       <c r="A193">
         <v>223</v>
       </c>
-      <c r="B193" t="s">
+      <c r="B193" s="1" t="s">
         <v>464</v>
       </c>
       <c r="C193">
@@ -8347,7 +8347,7 @@
       <c r="A194">
         <v>224</v>
       </c>
-      <c r="B194" t="s">
+      <c r="B194" s="1" t="s">
         <v>467</v>
       </c>
       <c r="C194">
@@ -8373,7 +8373,7 @@
       <c r="A195">
         <v>225</v>
       </c>
-      <c r="B195" t="s">
+      <c r="B195" s="1" t="s">
         <v>469</v>
       </c>
       <c r="C195">
@@ -8399,7 +8399,7 @@
       <c r="A196">
         <v>226</v>
       </c>
-      <c r="B196" t="s">
+      <c r="B196" s="1" t="s">
         <v>472</v>
       </c>
       <c r="C196">
@@ -8425,7 +8425,7 @@
       <c r="A197">
         <v>227</v>
       </c>
-      <c r="B197" t="s">
+      <c r="B197" s="1" t="s">
         <v>475</v>
       </c>
       <c r="C197">
@@ -8451,7 +8451,7 @@
       <c r="A198">
         <v>228</v>
       </c>
-      <c r="B198" t="s">
+      <c r="B198" s="1" t="s">
         <v>477</v>
       </c>
       <c r="C198">
@@ -8477,7 +8477,7 @@
       <c r="A199">
         <v>230</v>
       </c>
-      <c r="B199" t="s">
+      <c r="B199" s="1" t="s">
         <v>479</v>
       </c>
       <c r="C199">
@@ -8503,7 +8503,7 @@
       <c r="A200">
         <v>231</v>
       </c>
-      <c r="B200" t="s">
+      <c r="B200" s="1" t="s">
         <v>482</v>
       </c>
       <c r="C200">
@@ -8529,7 +8529,7 @@
       <c r="A201">
         <v>232</v>
       </c>
-      <c r="B201" t="s">
+      <c r="B201" s="1" t="s">
         <v>485</v>
       </c>
       <c r="C201">
@@ -8555,7 +8555,7 @@
       <c r="A202">
         <v>233</v>
       </c>
-      <c r="B202" t="s">
+      <c r="B202" s="1" t="s">
         <v>488</v>
       </c>
       <c r="C202">
@@ -8581,7 +8581,7 @@
       <c r="A203">
         <v>234</v>
       </c>
-      <c r="B203" t="s">
+      <c r="B203" s="1" t="s">
         <v>490</v>
       </c>
       <c r="C203">
@@ -8607,7 +8607,7 @@
       <c r="A204">
         <v>235</v>
       </c>
-      <c r="B204" t="s">
+      <c r="B204" s="1" t="s">
         <v>493</v>
       </c>
       <c r="C204">

</xml_diff>